<commit_message>
Get complex import test green
</commit_message>
<xml_diff>
--- a/tests/complex.xlsx
+++ b/tests/complex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grant/Sites/invoicing/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4FCB8B-788F-8540-B301-12F979A2D1E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0123BB68-D813-454C-A2F7-23DD5AFBA4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2860" yWindow="1920" windowWidth="28040" windowHeight="17440" xr2:uid="{316203B2-6E37-B24E-8594-CD512E76DFF9}"/>
+    <workbookView xWindow="17880" yWindow="8540" windowWidth="28040" windowHeight="17440" xr2:uid="{316203B2-6E37-B24E-8594-CD512E76DFF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -486,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF8D4C1-C401-A441-8697-8DB4DF205EA0}">
   <dimension ref="A2:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>